<commit_message>
You can see doll's status if you push C key.
</commit_message>
<xml_diff>
--- a/Documents/企画書関連/人形の能力値.xlsx
+++ b/Documents/企画書関連/人形の能力値.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="26">
   <si>
     <t>HP</t>
     <phoneticPr fontId="1"/>
@@ -150,83 +150,11 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>B</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>A</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>A</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>B</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>B</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>B</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>E</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>A+</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>E</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>E</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>D</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>B</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>B</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>D</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>C</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>E</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>D</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>A</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>C</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>A+</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -244,27 +172,11 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>C</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>D</t>
+    <t>A+</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
     <t>A-</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>C</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>A</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>B</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -288,15 +200,45 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFEC5652"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -304,13 +246,47 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -319,6 +295,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFEC5652"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -620,7 +601,7 @@
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -629,260 +610,261 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="B1" s="1" t="s">
+      <c r="A1" s="2"/>
+      <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="3" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A2" t="s">
+      <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D2" s="1" t="s">
+      <c r="B2" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="E2" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="F2" s="1" t="s">
+      <c r="E2" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2" s="5" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A3" t="s">
+      <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C3" s="1" t="s">
+      <c r="B3" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="E3" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="F3" s="1" t="s">
+      <c r="F5" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A6" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" s="6" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="1" t="s">
+      <c r="E6" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A8" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="E8" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A9" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A10" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A11" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F4" s="1" t="s">
+      <c r="B11" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F11" s="7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A12" s="2" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="D7" s="1" t="s">
+      <c r="B12" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="E12" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A13" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D13" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="E7" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A8" t="s">
-        <v>11</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A9" t="s">
-        <v>12</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A10" t="s">
-        <v>13</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A11" t="s">
-        <v>40</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A12" t="s">
-        <v>41</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A13" t="s">
-        <v>14</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>20</v>
+      <c r="E13" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="F13" s="8" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed bugs and add comment to Document.  Please enter the commit message for your changes. Lines starting
</commit_message>
<xml_diff>
--- a/Documents/企画書関連/人形の能力値.xlsx
+++ b/Documents/企画書関連/人形の能力値.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="46">
   <si>
     <t>HP</t>
     <phoneticPr fontId="1"/>
@@ -177,6 +177,461 @@
   </si>
   <si>
     <t>A-</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>E+</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>プラスやマイナスは能力的にはそのランクだが、</t>
+    <rPh sb="9" eb="12">
+      <t>ノウリョクテキ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>レベルアップ時の内部レベル補正が大きいか小さいかを意味する。</t>
+    <rPh sb="6" eb="7">
+      <t>ジ</t>
+    </rPh>
+    <rPh sb="8" eb="10">
+      <t>ナイブ</t>
+    </rPh>
+    <rPh sb="13" eb="15">
+      <t>ホセイ</t>
+    </rPh>
+    <rPh sb="16" eb="17">
+      <t>オオ</t>
+    </rPh>
+    <rPh sb="20" eb="21">
+      <t>チイ</t>
+    </rPh>
+    <rPh sb="25" eb="27">
+      <t>イミ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>例として、ゴリアテ人形と演奏家の人形は同程度のHPを持つが、</t>
+    <rPh sb="0" eb="1">
+      <t>レイ</t>
+    </rPh>
+    <rPh sb="9" eb="11">
+      <t>ニンギョウ</t>
+    </rPh>
+    <rPh sb="12" eb="15">
+      <t>エンソウカ</t>
+    </rPh>
+    <rPh sb="16" eb="18">
+      <t>ニンギョウ</t>
+    </rPh>
+    <rPh sb="19" eb="22">
+      <t>ドウテイド</t>
+    </rPh>
+    <rPh sb="26" eb="27">
+      <t>モ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>それを元に合成を行った場合はゴリアテを親にする人形の方が</t>
+    <rPh sb="3" eb="4">
+      <t>モト</t>
+    </rPh>
+    <rPh sb="5" eb="7">
+      <t>ゴウセイ</t>
+    </rPh>
+    <rPh sb="8" eb="9">
+      <t>オコナ</t>
+    </rPh>
+    <rPh sb="11" eb="13">
+      <t>バアイ</t>
+    </rPh>
+    <rPh sb="19" eb="20">
+      <t>オヤ</t>
+    </rPh>
+    <rPh sb="23" eb="25">
+      <t>ニンギョウ</t>
+    </rPh>
+    <rPh sb="26" eb="27">
+      <t>ホウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>微妙にHPが高くなる。</t>
+    <rPh sb="0" eb="2">
+      <t>ビミョウ</t>
+    </rPh>
+    <rPh sb="6" eb="7">
+      <t>タカ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>戦闘スタイル</t>
+    <rPh sb="0" eb="2">
+      <t>セントウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>戦闘スタイルの意味については、各パラメータの意味合い.txtも参照のこと。</t>
+    <rPh sb="0" eb="2">
+      <t>セントウ</t>
+    </rPh>
+    <rPh sb="7" eb="9">
+      <t>イミ</t>
+    </rPh>
+    <rPh sb="15" eb="16">
+      <t>カク</t>
+    </rPh>
+    <rPh sb="22" eb="25">
+      <t>イミア</t>
+    </rPh>
+    <rPh sb="31" eb="33">
+      <t>サンショウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>特技は全体的にあまり強くない。比較的高いHPと安定したパラメータで戦う。</t>
+    <rPh sb="0" eb="2">
+      <t>トクギ</t>
+    </rPh>
+    <rPh sb="3" eb="6">
+      <t>ゼンタイテキ</t>
+    </rPh>
+    <rPh sb="10" eb="11">
+      <t>ツヨ</t>
+    </rPh>
+    <rPh sb="15" eb="18">
+      <t>ヒカクテキ</t>
+    </rPh>
+    <rPh sb="18" eb="19">
+      <t>タカ</t>
+    </rPh>
+    <rPh sb="23" eb="25">
+      <t>アンテイ</t>
+    </rPh>
+    <rPh sb="33" eb="34">
+      <t>タタカ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>比較的高い攻撃と敏捷が武器。燃費は良いがHPが少ないのが難。</t>
+    <rPh sb="0" eb="3">
+      <t>ヒカクテキ</t>
+    </rPh>
+    <rPh sb="3" eb="4">
+      <t>タカ</t>
+    </rPh>
+    <rPh sb="5" eb="7">
+      <t>コウゲキ</t>
+    </rPh>
+    <rPh sb="8" eb="10">
+      <t>ビンショウ</t>
+    </rPh>
+    <rPh sb="11" eb="13">
+      <t>ブキ</t>
+    </rPh>
+    <rPh sb="14" eb="16">
+      <t>ネンピ</t>
+    </rPh>
+    <rPh sb="17" eb="18">
+      <t>ヨ</t>
+    </rPh>
+    <rPh sb="23" eb="24">
+      <t>スク</t>
+    </rPh>
+    <rPh sb="28" eb="29">
+      <t>ナン</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>HPと攻撃が高く、とても燃費が良い。しかしサポートや搦め手全般は苦手。</t>
+    <rPh sb="3" eb="5">
+      <t>コウゲキ</t>
+    </rPh>
+    <rPh sb="6" eb="7">
+      <t>タカ</t>
+    </rPh>
+    <rPh sb="12" eb="14">
+      <t>ネンピ</t>
+    </rPh>
+    <rPh sb="15" eb="16">
+      <t>ヨ</t>
+    </rPh>
+    <rPh sb="26" eb="27">
+      <t>カラ</t>
+    </rPh>
+    <rPh sb="28" eb="29">
+      <t>テ</t>
+    </rPh>
+    <rPh sb="29" eb="31">
+      <t>ゼンパン</t>
+    </rPh>
+    <rPh sb="32" eb="34">
+      <t>ニガテ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ゴリアテほどではないが高いHPと攻撃、敏捷も極めて高い。</t>
+    <rPh sb="11" eb="12">
+      <t>タカ</t>
+    </rPh>
+    <rPh sb="16" eb="18">
+      <t>コウゲキ</t>
+    </rPh>
+    <rPh sb="19" eb="21">
+      <t>ビンショウ</t>
+    </rPh>
+    <rPh sb="22" eb="23">
+      <t>キワ</t>
+    </rPh>
+    <rPh sb="25" eb="26">
+      <t>タカ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>高い敏捷と魔力でサポートに徹する。HPが低いのが難点。</t>
+    <rPh sb="0" eb="1">
+      <t>タカ</t>
+    </rPh>
+    <rPh sb="2" eb="4">
+      <t>ビンショウ</t>
+    </rPh>
+    <rPh sb="5" eb="7">
+      <t>マリョク</t>
+    </rPh>
+    <rPh sb="13" eb="14">
+      <t>テッ</t>
+    </rPh>
+    <rPh sb="20" eb="21">
+      <t>ヒク</t>
+    </rPh>
+    <rPh sb="24" eb="26">
+      <t>ナンテン</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>サポートはかなり得意だが、攻撃面は絶望的。打たれ強いので回復役向き。</t>
+    <rPh sb="8" eb="10">
+      <t>トクイ</t>
+    </rPh>
+    <rPh sb="13" eb="15">
+      <t>コウゲキ</t>
+    </rPh>
+    <rPh sb="15" eb="16">
+      <t>メン</t>
+    </rPh>
+    <rPh sb="17" eb="20">
+      <t>ゼツボウテキ</t>
+    </rPh>
+    <rPh sb="21" eb="22">
+      <t>ウ</t>
+    </rPh>
+    <rPh sb="24" eb="25">
+      <t>ヅヨ</t>
+    </rPh>
+    <rPh sb="28" eb="30">
+      <t>カイフク</t>
+    </rPh>
+    <rPh sb="30" eb="31">
+      <t>ヤク</t>
+    </rPh>
+    <rPh sb="31" eb="32">
+      <t>ム</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>魔力が全人形中最高で、比較的バランスも良い。素早さが低いのが欠点。</t>
+    <rPh sb="0" eb="2">
+      <t>マリョク</t>
+    </rPh>
+    <rPh sb="3" eb="4">
+      <t>ゼン</t>
+    </rPh>
+    <rPh sb="4" eb="6">
+      <t>ニンギョウ</t>
+    </rPh>
+    <rPh sb="6" eb="7">
+      <t>チュウ</t>
+    </rPh>
+    <rPh sb="7" eb="9">
+      <t>サイコウ</t>
+    </rPh>
+    <rPh sb="11" eb="14">
+      <t>ヒカクテキ</t>
+    </rPh>
+    <rPh sb="19" eb="20">
+      <t>ヨ</t>
+    </rPh>
+    <rPh sb="22" eb="24">
+      <t>スバヤ</t>
+    </rPh>
+    <rPh sb="26" eb="27">
+      <t>ヒク</t>
+    </rPh>
+    <rPh sb="30" eb="32">
+      <t>ケッテン</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Lv1にしては技巧がかなり高く、援護射撃向き。魔力枯渇には注意が必要。</t>
+    <rPh sb="7" eb="9">
+      <t>ギコウ</t>
+    </rPh>
+    <rPh sb="13" eb="14">
+      <t>タカ</t>
+    </rPh>
+    <rPh sb="16" eb="18">
+      <t>エンゴ</t>
+    </rPh>
+    <rPh sb="18" eb="20">
+      <t>シャゲキ</t>
+    </rPh>
+    <rPh sb="20" eb="21">
+      <t>ム</t>
+    </rPh>
+    <rPh sb="23" eb="25">
+      <t>マリョク</t>
+    </rPh>
+    <rPh sb="25" eb="27">
+      <t>コカツ</t>
+    </rPh>
+    <rPh sb="29" eb="31">
+      <t>チュウイ</t>
+    </rPh>
+    <rPh sb="32" eb="34">
+      <t>ヒツヨウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>直接攻撃は苦手だが、平均して高い能力。リベンジ系の特徴的な特技。</t>
+    <rPh sb="0" eb="2">
+      <t>チョクセツ</t>
+    </rPh>
+    <rPh sb="2" eb="4">
+      <t>コウゲキ</t>
+    </rPh>
+    <rPh sb="5" eb="7">
+      <t>ニガテ</t>
+    </rPh>
+    <rPh sb="10" eb="12">
+      <t>ヘイキン</t>
+    </rPh>
+    <rPh sb="14" eb="15">
+      <t>タカ</t>
+    </rPh>
+    <rPh sb="16" eb="18">
+      <t>ノウリョク</t>
+    </rPh>
+    <rPh sb="23" eb="24">
+      <t>ケイ</t>
+    </rPh>
+    <rPh sb="25" eb="28">
+      <t>トクチョウテキ</t>
+    </rPh>
+    <rPh sb="29" eb="31">
+      <t>トクギ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>援護射撃・サポートの両方が得意で、攻撃も悪くない。ただしHPは最低。</t>
+    <rPh sb="0" eb="2">
+      <t>エンゴ</t>
+    </rPh>
+    <rPh sb="2" eb="4">
+      <t>シャゲキ</t>
+    </rPh>
+    <rPh sb="10" eb="12">
+      <t>リョウホウ</t>
+    </rPh>
+    <rPh sb="13" eb="15">
+      <t>トクイ</t>
+    </rPh>
+    <rPh sb="17" eb="19">
+      <t>コウゲキ</t>
+    </rPh>
+    <rPh sb="20" eb="21">
+      <t>ワル</t>
+    </rPh>
+    <rPh sb="31" eb="33">
+      <t>サイテイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>攻撃・技巧がトップクラス。通常攻撃も援護射撃もお手の物。HPは低め。</t>
+    <rPh sb="0" eb="2">
+      <t>コウゲキ</t>
+    </rPh>
+    <rPh sb="3" eb="5">
+      <t>ギコウ</t>
+    </rPh>
+    <rPh sb="13" eb="15">
+      <t>ツウジョウ</t>
+    </rPh>
+    <rPh sb="15" eb="17">
+      <t>コウゲキ</t>
+    </rPh>
+    <rPh sb="18" eb="20">
+      <t>エンゴ</t>
+    </rPh>
+    <rPh sb="20" eb="22">
+      <t>シャゲキ</t>
+    </rPh>
+    <rPh sb="24" eb="27">
+      <t>テノモノ</t>
+    </rPh>
+    <rPh sb="31" eb="32">
+      <t>ヒク</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>打たれ強く、サポートが得意。技巧が高く搦め手を得意とする。燃費は悪い。</t>
+    <rPh sb="0" eb="1">
+      <t>ウ</t>
+    </rPh>
+    <rPh sb="3" eb="4">
+      <t>ヅヨ</t>
+    </rPh>
+    <rPh sb="11" eb="13">
+      <t>トクイ</t>
+    </rPh>
+    <rPh sb="14" eb="16">
+      <t>ギコウ</t>
+    </rPh>
+    <rPh sb="17" eb="18">
+      <t>タカ</t>
+    </rPh>
+    <rPh sb="19" eb="20">
+      <t>カラ</t>
+    </rPh>
+    <rPh sb="21" eb="22">
+      <t>テ</t>
+    </rPh>
+    <rPh sb="23" eb="25">
+      <t>トクイ</t>
+    </rPh>
+    <rPh sb="29" eb="31">
+      <t>ネンピ</t>
+    </rPh>
+    <rPh sb="32" eb="33">
+      <t>ワル</t>
+    </rPh>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -238,7 +693,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -261,11 +716,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -289,6 +753,10 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="標準" xfId="0" builtinId="0"/>
@@ -598,273 +1066,344 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:H20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K4" sqref="K4"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="2" max="6" width="5.625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="67.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A1" s="2"/>
-      <c r="B1" s="3" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="G1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A2" s="2"/>
+      <c r="B2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F2" s="3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A2" s="2" t="s">
+      <c r="G2" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="H2" s="10"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C2" s="4" t="s">
+      <c r="B3" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D3" s="4" t="s">
         <v>17</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C3" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="D3" s="8" t="s">
-        <v>15</v>
       </c>
       <c r="E3" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="F3" s="7" t="s">
+      <c r="F3" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="G3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="7" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A4" s="2" t="s">
+      <c r="D4" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="G4" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A5" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B5" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C5" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D5" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="E4" s="7" t="s">
+      <c r="E5" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="F4" s="8" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A5" s="2" t="s">
+      <c r="F5" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="G5" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A6" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B6" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="D5" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="E5" s="6" t="s">
+      <c r="C6" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="F5" s="4" t="s">
+      <c r="F6" s="4" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A6" s="2" t="s">
+      <c r="G6" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A7" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="B7" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="C7" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="D7" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="E6" s="6" t="s">
+      <c r="E7" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="F6" s="5" t="s">
+      <c r="F7" s="5" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A7" s="2" t="s">
+      <c r="G7" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A8" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C7" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="D7" s="7" t="s">
+      <c r="B8" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="E7" s="5" t="s">
+      <c r="E8" s="5" t="s">
         <v>18</v>
-      </c>
-      <c r="F7" s="4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A8" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B8" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="D8" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="E8" s="8" t="s">
-        <v>15</v>
       </c>
       <c r="F8" s="4" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G8" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A9" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="E9" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="G9" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A10" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="7" t="s">
+      <c r="B10" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="C9" s="6" t="s">
+      <c r="C10" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="D9" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="E9" s="7" t="s">
+      <c r="D10" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="E10" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="F9" s="6" t="s">
+      <c r="F10" s="6" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A10" s="2" t="s">
+      <c r="G10" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A11" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C10" s="4" t="s">
+      <c r="B11" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" s="4" t="s">
         <v>16</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="E10" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="F10" s="4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A11" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>18</v>
       </c>
       <c r="D11" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="E11" s="4" t="s">
+      <c r="E11" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="F11" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="F11" s="7" t="s">
+      <c r="G11" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A12" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F12" s="7" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A12" s="2" t="s">
+      <c r="G12" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A13" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B12" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C12" s="6" t="s">
+      <c r="B13" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C13" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="D12" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="E12" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="F12" s="4" t="s">
+      <c r="D13" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="E13" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="F13" s="4" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A13" s="2" t="s">
+      <c r="G13" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A14" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B13" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C13" s="4" t="s">
+      <c r="B14" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C14" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="D13" s="7" t="s">
+      <c r="D14" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="E13" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="F13" s="8" t="s">
-        <v>15</v>
+      <c r="E14" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="F14" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="G14" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A16" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A17" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A18" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A19" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A20" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>